<commit_message>
Update issue 235 SALVIA:   Refactor index_fetcher.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,6 +70,10 @@
   </si>
   <si>
     <t>v1254</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1282</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -134,7 +138,61 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -900,13 +958,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -918,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -940,7 +998,9 @@
       <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -959,7 +1019,9 @@
       <c r="E2" s="1">
         <v>10467</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>10031</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -978,7 +1040,9 @@
       <c r="E3" s="1">
         <v>10442</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>10058</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -997,7 +1061,9 @@
       <c r="E4" s="1">
         <v>10466</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>10015</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1016,7 +1082,9 @@
       <c r="E5" s="1">
         <v>10429</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>10048</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1035,7 +1103,9 @@
       <c r="E6" s="1">
         <v>10443</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>10141</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1054,7 +1124,9 @@
       <c r="E7" s="1">
         <v>10495</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>10045</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1073,7 +1145,9 @@
       <c r="E8" s="1">
         <v>10452</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>10021</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1092,7 +1166,9 @@
       <c r="E9" s="1">
         <v>10537</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>10039</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1111,7 +1187,9 @@
       <c r="E10" s="1">
         <v>10539</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>10043</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1130,7 +1208,9 @@
       <c r="E11" s="1">
         <v>10471</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>10041</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1153,9 +1233,9 @@
         <f t="shared" si="0"/>
         <v>10474.1</v>
       </c>
-      <c r="F12" s="3" t="e">
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>10048.200000000001</v>
       </c>
       <c r="G12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -1182,9 +1262,9 @@
         <f t="shared" si="2"/>
         <v>1472.3222222222223</v>
       </c>
-      <c r="F13" s="3" t="e">
+      <c r="F13" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1224.4000000000005</v>
       </c>
       <c r="G13" s="3" t="e">
         <f t="shared" si="2"/>
@@ -1210,9 +1290,9 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="e">
+      <c r="F14" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.99999999999999867</v>
       </c>
       <c r="G14" s="1" t="e">
         <f t="shared" si="4"/>
@@ -1238,9 +1318,9 @@
         <f>D12/E12</f>
         <v>1.104887293419005</v>
       </c>
-      <c r="F15" s="1" t="e">
-        <f>D12/F12</f>
-        <v>#DIV/0!</v>
+      <c r="F15" s="1">
+        <f>E12/F12</f>
+        <v>1.042385700921558</v>
       </c>
       <c r="G15" s="1" t="e">
         <f>F12/G12</f>
@@ -1266,9 +1346,9 @@
         <f>B12/E12</f>
         <v>1.1782778472613398</v>
       </c>
-      <c r="F16" s="1" t="e">
+      <c r="F16" s="1">
         <f>B12/F12</f>
-        <v>#DIV/0!</v>
+        <v>1.2282199796978561</v>
       </c>
       <c r="G16" s="1" t="e">
         <f>B12/G12</f>
@@ -1297,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1319,7 +1399,9 @@
       <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1338,7 +1420,9 @@
       <c r="E2" s="1">
         <v>7602</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>7530</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1357,7 +1441,9 @@
       <c r="E3" s="1">
         <v>7629</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>7551</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1376,7 +1462,9 @@
       <c r="E4" s="1">
         <v>7600</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>7535</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1395,7 +1483,9 @@
       <c r="E5" s="1">
         <v>7584</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>7513</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1414,7 +1504,9 @@
       <c r="E6" s="1">
         <v>7590</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>7517</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1433,7 +1525,9 @@
       <c r="E7" s="1">
         <v>7623</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>7538</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1452,7 +1546,9 @@
       <c r="E8" s="1">
         <v>7604</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>7553</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1471,7 +1567,9 @@
       <c r="E9" s="1">
         <v>7629</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>7544</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1490,7 +1588,9 @@
       <c r="E10" s="1">
         <v>7611</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>7586</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1509,7 +1609,9 @@
       <c r="E11" s="1">
         <v>7627</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>7573</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1532,9 +1634,9 @@
         <f t="shared" si="0"/>
         <v>7609.9</v>
       </c>
-      <c r="F12" s="3" t="e">
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>7544</v>
       </c>
       <c r="G12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -1561,9 +1663,9 @@
         <f t="shared" si="1"/>
         <v>272.98888888888888</v>
       </c>
-      <c r="F13" s="3" t="e">
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>526.44444444444446</v>
       </c>
       <c r="G13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -1589,9 +1691,9 @@
         <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
         <v>0.98060608956061501</v>
       </c>
-      <c r="F14" s="1" t="e">
+      <c r="F14" s="1">
         <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999994274217585</v>
       </c>
       <c r="G14" s="1" t="e">
         <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
@@ -1617,9 +1719,9 @@
         <f>D12/E12</f>
         <v>1.0029041117491688</v>
       </c>
-      <c r="F15" s="1" t="e">
-        <f>D12/F12</f>
-        <v>#DIV/0!</v>
+      <c r="F15" s="1">
+        <f>E12/F12</f>
+        <v>1.0087354188759279</v>
       </c>
       <c r="G15" s="1" t="e">
         <f>F12/G12</f>
@@ -1645,9 +1747,9 @@
         <f>B12/E12</f>
         <v>1.0342711467956216</v>
       </c>
-      <c r="F16" s="1" t="e">
+      <c r="F16" s="1">
         <f>B12/F12</f>
-        <v>#DIV/0!</v>
+        <v>1.0433059384941674</v>
       </c>
       <c r="G16" s="1" t="e">
         <f>B12/G12</f>
@@ -1657,13 +1759,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update issue 243 SALVIA:   Put window handle into renderer_parameters.   Now texture hold surface pointers but not vector of surface. (STILL RUNNING ERROR)   Remove unused hdev for renderer creating.   Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,6 +74,10 @@
   </si>
   <si>
     <t>v1282</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1289</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -138,61 +142,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -958,13 +908,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -976,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1001,7 +951,9 @@
       <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -1022,7 +974,9 @@
       <c r="F2" s="1">
         <v>10031</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>10176</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1043,7 +997,9 @@
       <c r="F3" s="1">
         <v>10058</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <v>10206</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1064,7 +1020,9 @@
       <c r="F4" s="1">
         <v>10015</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>10194</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1085,7 +1043,9 @@
       <c r="F5" s="1">
         <v>10048</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>10139</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1106,7 +1066,9 @@
       <c r="F6" s="1">
         <v>10141</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>10157</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1127,7 +1089,9 @@
       <c r="F7" s="1">
         <v>10045</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>10184</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1148,7 +1112,9 @@
       <c r="F8" s="1">
         <v>10021</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>10201</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1169,7 +1135,9 @@
       <c r="F9" s="1">
         <v>10039</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>10175</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1190,7 +1158,9 @@
       <c r="F10" s="1">
         <v>10043</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>10125</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1211,7 +1181,9 @@
       <c r="F11" s="1">
         <v>10041</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>10187</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1237,9 +1209,9 @@
         <f t="shared" si="0"/>
         <v>10048.200000000001</v>
       </c>
-      <c r="G12" s="3" t="e">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>10174.4</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1266,9 +1238,9 @@
         <f t="shared" si="2"/>
         <v>1224.4000000000005</v>
       </c>
-      <c r="G13" s="3" t="e">
+      <c r="G13" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>704.48888888888894</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1294,9 +1266,9 @@
         <f t="shared" si="4"/>
         <v>0.99999999999999867</v>
       </c>
-      <c r="G14" s="1" t="e">
+      <c r="G14" s="1">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.99999993108443863</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1322,9 +1294,9 @@
         <f>E12/F12</f>
         <v>1.042385700921558</v>
       </c>
-      <c r="G15" s="1" t="e">
+      <c r="G15" s="1">
         <f>F12/G12</f>
-        <v>#DIV/0!</v>
+        <v>0.98759632017612842</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1350,9 +1322,9 @@
         <f>B12/F12</f>
         <v>1.2282199796978561</v>
       </c>
-      <c r="G16" s="1" t="e">
+      <c r="G16" s="1">
         <f>B12/G12</f>
-        <v>#DIV/0!</v>
+        <v>1.212985532316402</v>
       </c>
     </row>
   </sheetData>
@@ -1377,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1402,7 +1374,9 @@
       <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -1423,7 +1397,9 @@
       <c r="F2" s="1">
         <v>7530</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>7683</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1444,7 +1420,9 @@
       <c r="F3" s="1">
         <v>7551</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <v>7657</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1465,7 +1443,9 @@
       <c r="F4" s="1">
         <v>7535</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>7648</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1486,7 +1466,9 @@
       <c r="F5" s="1">
         <v>7513</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>7612</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1507,7 +1489,9 @@
       <c r="F6" s="1">
         <v>7517</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>7716</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1528,7 +1512,9 @@
       <c r="F7" s="1">
         <v>7538</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>7690</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1549,7 +1535,9 @@
       <c r="F8" s="1">
         <v>7553</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>7631</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1570,7 +1558,9 @@
       <c r="F9" s="1">
         <v>7544</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>7615</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1591,7 +1581,9 @@
       <c r="F10" s="1">
         <v>7586</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>7645</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1612,7 +1604,9 @@
       <c r="F11" s="1">
         <v>7573</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>7643</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1638,9 +1632,9 @@
         <f t="shared" si="0"/>
         <v>7544</v>
       </c>
-      <c r="G12" s="3" t="e">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>7654</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1667,9 +1661,9 @@
         <f t="shared" si="1"/>
         <v>526.44444444444446</v>
       </c>
-      <c r="G13" s="3" t="e">
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1115.7777777777778</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1695,9 +1689,9 @@
         <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
         <v>0.99999994274217585</v>
       </c>
-      <c r="G14" s="1" t="e">
+      <c r="G14" s="1">
         <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999977450891742</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1723,9 +1717,9 @@
         <f>E12/F12</f>
         <v>1.0087354188759279</v>
       </c>
-      <c r="G15" s="1" t="e">
+      <c r="G15" s="1">
         <f>F12/G12</f>
-        <v>#DIV/0!</v>
+        <v>0.98562842957930497</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1751,21 +1745,21 @@
         <f>B12/F12</f>
         <v>1.0433059384941674</v>
       </c>
-      <c r="G16" s="1" t="e">
+      <c r="G16" s="1">
         <f>B12/G12</f>
-        <v>#DIV/0!</v>
+        <v>1.0283119937287692</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update issue 260 Update peformance documents.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,10 @@
   </si>
   <si>
     <t>v1410</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1419</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1048,15 +1052,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1087,8 +1091,11 @@
       <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1119,8 +1126,11 @@
       <c r="J2" s="1">
         <v>8400</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>8415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1151,8 +1161,11 @@
       <c r="J3" s="1">
         <v>8382</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>8327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1183,8 +1196,11 @@
       <c r="J4" s="1">
         <v>8397</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>8288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1215,8 +1231,11 @@
       <c r="J5" s="1">
         <v>8364</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>8295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1247,8 +1266,11 @@
       <c r="J6" s="1">
         <v>8354</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>8285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1279,8 +1301,11 @@
       <c r="J7" s="1">
         <v>8368</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>8292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1311,8 +1336,11 @@
       <c r="J8" s="1">
         <v>8383</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>8333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1343,8 +1371,11 @@
       <c r="J9" s="1">
         <v>8398</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>8308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1375,8 +1406,11 @@
       <c r="J10" s="1">
         <v>8383</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>8271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1407,8 +1441,11 @@
       <c r="J11" s="1">
         <v>8368</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>8272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1437,7 +1474,7 @@
         <v>10174.4</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12:J12" si="2">AVERAGE(H2:H11)</f>
+        <f t="shared" ref="H12:K12" si="2">AVERAGE(H2:H11)</f>
         <v>8442.4</v>
       </c>
       <c r="I12" s="3">
@@ -1448,8 +1485,12 @@
         <f t="shared" si="2"/>
         <v>8379.7000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K12" s="3">
+        <f t="shared" si="2"/>
+        <v>8308.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1489,8 +1530,12 @@
         <f>_xlfn.VAR.S(J2:J11)</f>
         <v>250.45555555555561</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <f>_xlfn.VAR.S(K2:K11)</f>
+        <v>1827.8222222222223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1547,7 @@
         <v>0.9999999869691466</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:J14" si="5">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <f t="shared" ref="D14:K14" si="5">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999999999889</v>
       </c>
       <c r="E14" s="1">
@@ -1529,8 +1574,12 @@
         <f t="shared" si="5"/>
         <v>0.99999936755718299</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99959879047769007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1538,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:J15" si="6">B12/C12</f>
+        <f t="shared" ref="C15:K15" si="6">B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
       <c r="D15" s="1">
@@ -1569,8 +1618,12 @@
         <f t="shared" si="6"/>
         <v>1.0159790923302743</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <f t="shared" si="6"/>
+        <v>1.0085573983583276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1609,10 +1662,14 @@
         <f>B12/J12</f>
         <v>1.4727734883110373</v>
       </c>
+      <c r="K16" s="1">
+        <f>B12/K12</f>
+        <v>1.4853765977420985</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:J16">
+  <conditionalFormatting sqref="B15:K16">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -1630,15 +1687,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1666,8 +1723,11 @@
       <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1695,8 +1755,11 @@
       <c r="I2" s="1">
         <v>6383</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <v>6422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1724,8 +1787,11 @@
       <c r="I3" s="1">
         <v>6377</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>6327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1753,8 +1819,11 @@
       <c r="I4" s="1">
         <v>6357</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>6296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1782,8 +1851,11 @@
       <c r="I5" s="1">
         <v>6363</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>6329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1811,8 +1883,11 @@
       <c r="I6" s="1">
         <v>6390</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>6281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1840,8 +1915,11 @@
       <c r="I7" s="1">
         <v>6360</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>6304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1869,8 +1947,11 @@
       <c r="I8" s="1">
         <v>6365</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <v>6366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1898,8 +1979,11 @@
       <c r="I9" s="1">
         <v>6413</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>6346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1927,8 +2011,11 @@
       <c r="I10" s="1">
         <v>6378</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>6360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1956,8 +2043,11 @@
       <c r="I11" s="1">
         <v>6391</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <v>6326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1991,8 +2081,11 @@
       <c r="I12" s="1">
         <v>6355</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <v>6277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2028,8 +2121,12 @@
         <f t="shared" si="2"/>
         <v>302.45555555555558</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f t="shared" ref="J13" si="3">_xlfn.VAR.S(J2:J11)</f>
+        <v>1650.0111111111112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2064,8 +2161,12 @@
         <f>1-_xlfn.T.TEST(H2:H11,I2:I11,2,3)</f>
         <v>0.99981320279925834</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <f>1-_xlfn.T.TEST(I2:I11,J2:J11,2,3)</f>
+        <v>0.98922245269585052</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2073,35 +2174,39 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:I15" si="3">B12/C12</f>
+        <f t="shared" ref="C15:J15" si="4">B12/C12</f>
         <v>1.0128558192206722</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0181865828092242</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0029041117491688</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0087354188759279</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.98562842957930497</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1933270969753664</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0092840283241542</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0124263183049227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2136,10 +2241,14 @@
         <f>B12/I12</f>
         <v>1.2385051140833989</v>
       </c>
+      <c r="J16" s="1">
+        <f>B12/J12</f>
+        <v>1.2538951728532739</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:I16">
+  <conditionalFormatting sqref="B15:J16">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update issue 260 Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,10 @@
   </si>
   <si>
     <t>v1419</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1423</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1052,15 +1056,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1094,8 +1098,11 @@
       <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1129,8 +1136,11 @@
       <c r="K2" s="1">
         <v>8415</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L2" s="1">
+        <v>7242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1164,8 +1174,11 @@
       <c r="K3" s="1">
         <v>8327</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L3" s="1">
+        <v>7229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1199,8 +1212,11 @@
       <c r="K4" s="1">
         <v>8288</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L4" s="1">
+        <v>7226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1234,8 +1250,11 @@
       <c r="K5" s="1">
         <v>8295</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L5" s="1">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1269,8 +1288,11 @@
       <c r="K6" s="1">
         <v>8285</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>7204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1304,8 +1326,11 @@
       <c r="K7" s="1">
         <v>8292</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>7226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1339,8 +1364,11 @@
       <c r="K8" s="1">
         <v>8333</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>7212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1374,8 +1402,11 @@
       <c r="K9" s="1">
         <v>8308</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <v>7262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1409,8 +1440,11 @@
       <c r="K10" s="1">
         <v>8271</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <v>7229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1444,8 +1478,11 @@
       <c r="K11" s="1">
         <v>8272</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <v>7264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1489,8 +1526,12 @@
         <f t="shared" si="2"/>
         <v>8308.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L12" s="3">
+        <f t="shared" ref="L12" si="3">AVERAGE(L2:L11)</f>
+        <v>7234.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1499,23 +1540,23 @@
         <v>1875.377777777778</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="C13:G13" si="3">_xlfn.VAR.S(C2:C11)</f>
+        <f t="shared" ref="C13:G13" si="4">_xlfn.VAR.S(C2:C11)</f>
         <v>1924.1777777777779</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13" si="4">_xlfn.VAR.S(D2:D11)</f>
+        <f t="shared" ref="D13" si="5">_xlfn.VAR.S(D2:D11)</f>
         <v>682.01111111111118</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1472.3222222222223</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1224.4000000000005</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>704.48888888888894</v>
       </c>
       <c r="H13" s="3">
@@ -1534,8 +1575,12 @@
         <f>_xlfn.VAR.S(K2:K11)</f>
         <v>1827.8222222222223</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L13" s="3">
+        <f>_xlfn.VAR.S(L2:L11)</f>
+        <v>411.51111111111118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1547,39 +1592,43 @@
         <v>0.9999999869691466</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:K14" si="5">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <f t="shared" ref="D14:L14" si="6">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999999999889</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99999999999999867</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99999993108443863</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99999999999999278</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.96439230163877454</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99999936755718299</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.99959879047769007</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L14" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1587,43 +1636,47 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:K15" si="6">B12/C12</f>
+        <f t="shared" ref="C15:L15" si="7">B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0499883346150856</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.104887293419005</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.042385700921558</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.98759632017612842</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2051549322467545</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.9916369103551963</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0159790923302743</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0085573983583276</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="L15" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1484215182175044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1666,10 +1719,14 @@
         <f>B12/K12</f>
         <v>1.4853765977420985</v>
       </c>
+      <c r="L16" s="1">
+        <f>B12/L12</f>
+        <v>1.7058384475037318</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:K16">
+  <conditionalFormatting sqref="B15:L16">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -1687,15 +1744,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1726,8 +1783,11 @@
       <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1758,8 +1818,11 @@
       <c r="J2" s="1">
         <v>6422</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>5249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1790,8 +1853,11 @@
       <c r="J3" s="1">
         <v>6327</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1822,8 +1888,11 @@
       <c r="J4" s="1">
         <v>6296</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>5073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1854,8 +1923,11 @@
       <c r="J5" s="1">
         <v>6329</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>5055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1886,8 +1958,11 @@
       <c r="J6" s="1">
         <v>6281</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>5051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1918,8 +1993,11 @@
       <c r="J7" s="1">
         <v>6304</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1950,8 +2028,11 @@
       <c r="J8" s="1">
         <v>6366</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1982,8 +2063,11 @@
       <c r="J9" s="1">
         <v>6346</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>5044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2014,8 +2098,11 @@
       <c r="J10" s="1">
         <v>6360</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>5058</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2046,8 +2133,11 @@
       <c r="J11" s="1">
         <v>6326</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>5077</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2084,8 +2174,11 @@
       <c r="J12" s="1">
         <v>6277</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>5119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2122,11 +2215,15 @@
         <v>302.45555555555558</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" ref="J13" si="3">_xlfn.VAR.S(J2:J11)</f>
+        <f t="shared" ref="J13:K13" si="3">_xlfn.VAR.S(J2:J11)</f>
         <v>1650.0111111111112</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <f t="shared" si="3"/>
+        <v>3637.9555555555553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2165,8 +2262,12 @@
         <f>1-_xlfn.T.TEST(I2:I11,J2:J11,2,3)</f>
         <v>0.98922245269585052</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K14" s="1">
+        <f>1-_xlfn.T.TEST(J2:J11,K2:K11,2,3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:J15" si="4">B12/C12</f>
+        <f t="shared" ref="C15:K15" si="4">B12/C12</f>
         <v>1.0128558192206722</v>
       </c>
       <c r="D15" s="1">
@@ -2205,8 +2306,12 @@
         <f t="shared" si="4"/>
         <v>1.0124263183049227</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.2262160578237937</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2245,10 +2350,14 @@
         <f>B12/J12</f>
         <v>1.2538951728532739</v>
       </c>
+      <c r="K16" s="1">
+        <f>B12/K12</f>
+        <v>1.5375463957804258</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:J16">
+  <conditionalFormatting sqref="B15:K16">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update issue 261 Add bm_collect.py to get performance data automatically. Update performance document for v1469
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="2175" yWindow="135" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,13 @@
   <si>
     <t>v1458</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1468</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1469</t>
   </si>
 </sst>
 </file>
@@ -625,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1026,15 +1033,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1086,8 +1093,14 @@
       <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1139,8 +1152,14 @@
       <c r="Q2" s="1">
         <v>5411</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R2" s="1">
+        <v>4755</v>
+      </c>
+      <c r="S2" s="1">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1192,8 +1211,14 @@
       <c r="Q3" s="1">
         <v>5380</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R3" s="1">
+        <v>4764</v>
+      </c>
+      <c r="S3" s="1">
+        <v>4591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1245,8 +1270,14 @@
       <c r="Q4" s="1">
         <v>5331</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R4" s="1">
+        <v>4770</v>
+      </c>
+      <c r="S4" s="1">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1298,8 +1329,14 @@
       <c r="Q5" s="1">
         <v>5336</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R5" s="1">
+        <v>4754</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1351,8 +1388,14 @@
       <c r="Q6" s="1">
         <v>5316</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <v>4765</v>
+      </c>
+      <c r="S6" s="1">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1404,8 +1447,14 @@
       <c r="Q7" s="1">
         <v>5414</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R7" s="1">
+        <v>4766</v>
+      </c>
+      <c r="S7" s="1">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1457,8 +1506,14 @@
       <c r="Q8" s="1">
         <v>5387</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R8" s="1">
+        <v>4753</v>
+      </c>
+      <c r="S8" s="1">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1510,8 +1565,14 @@
       <c r="Q9" s="1">
         <v>5349</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R9" s="1">
+        <v>4753</v>
+      </c>
+      <c r="S9" s="1">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1563,8 +1624,14 @@
       <c r="Q10" s="1">
         <v>5339</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R10" s="1">
+        <v>4754</v>
+      </c>
+      <c r="S10" s="1">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1616,8 +1683,14 @@
       <c r="Q11" s="1">
         <v>5324</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R11" s="1">
+        <v>4768</v>
+      </c>
+      <c r="S11" s="1">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1685,8 +1758,16 @@
         <f t="shared" si="5"/>
         <v>5358.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R12" s="3">
+        <f t="shared" ref="R12:S12" si="6">AVERAGE(R2:R11)</f>
+        <v>4760.2</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" si="6"/>
+        <v>4581.8999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1695,67 +1776,75 @@
         <v>1875.377777777778</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="C13:G13" si="6">_xlfn.VAR.S(C2:C11)</f>
+        <f t="shared" ref="C13:G13" si="7">_xlfn.VAR.S(C2:C11)</f>
         <v>1924.1777777777779</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13" si="7">_xlfn.VAR.S(D2:D11)</f>
+        <f t="shared" ref="D13" si="8">_xlfn.VAR.S(D2:D11)</f>
         <v>682.01111111111118</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1472.3222222222223</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1224.4000000000005</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>704.48888888888894</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13:M13" si="8">_xlfn.VAR.S(H2:H11)</f>
+        <f t="shared" ref="H13:M13" si="9">_xlfn.VAR.S(H2:H11)</f>
         <v>7530.9333333333325</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1657.377777777778</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>250.45555555555561</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1827.8222222222223</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>411.51111111111118</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>421.51111111111118</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" ref="N13:O13" si="9">_xlfn.VAR.S(N2:N11)</f>
+        <f t="shared" ref="N13:O13" si="10">_xlfn.VAR.S(N2:N11)</f>
         <v>183.56666666666669</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>194.23333333333335</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" ref="P13:Q13" si="10">_xlfn.VAR.S(P2:P11)</f>
+        <f t="shared" ref="P13:Q13" si="11">_xlfn.VAR.S(P2:P11)</f>
         <v>1109.5111111111109</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1315.5666666666666</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R13" s="3">
+        <f t="shared" ref="R13:S13" si="12">_xlfn.VAR.S(R2:R11)</f>
+        <v>48.4</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" si="12"/>
+        <v>110.32222222222222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1767,63 +1856,71 @@
         <v>0.9999999869691466</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:Q14" si="11">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <f t="shared" ref="D14:S14" si="13">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999999999889</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999867</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999993108443863</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999278</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.96439230163877454</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999936755718299</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99959879047769007</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999999624907909</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999745648</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R14" s="1">
+        <f t="shared" si="13"/>
+        <v>0.99999999999957156</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1831,67 +1928,75 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:Q15" si="12">B12/C12</f>
+        <f t="shared" ref="C15:S15" si="14">B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0499883346150856</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.104887293419005</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.042385700921558</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.98759632017612842</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.2051549322467545</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.9916369103551963</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0159790923302743</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0085573983583276</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.1484215182175044</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0354955058109578</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.1168694150934348</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0806744173994161</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0304211613086973</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0483512792281711</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="R15" s="1">
+        <f t="shared" si="14"/>
+        <v>1.1257300113440611</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="14"/>
+        <v>1.0389139876470461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1958,10 +2063,18 @@
         <f>B12/Q12</f>
         <v>2.3030585776400994</v>
       </c>
+      <c r="R16" s="1">
+        <f>B12/R12</f>
+        <v>2.5926221587328264</v>
+      </c>
+      <c r="S16" s="1">
+        <f>B12/S12</f>
+        <v>2.6935114253912134</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:Q16">
+  <conditionalFormatting sqref="B15:S16">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -1979,15 +2092,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="J19" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2036,8 +2149,14 @@
       <c r="P1" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2086,8 +2205,14 @@
       <c r="P2" s="1">
         <v>3505</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1">
+        <v>3772</v>
+      </c>
+      <c r="R2" s="1">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2136,8 +2261,14 @@
       <c r="P3" s="1">
         <v>3514</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1">
+        <v>3758</v>
+      </c>
+      <c r="R3" s="1">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2186,8 +2317,14 @@
       <c r="P4" s="1">
         <v>3532</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1">
+        <v>3769</v>
+      </c>
+      <c r="R4" s="1">
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2236,8 +2373,14 @@
       <c r="P5" s="1">
         <v>3500</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1">
+        <v>3773</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2286,8 +2429,14 @@
       <c r="P6" s="1">
         <v>3491</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q6" s="1">
+        <v>3759</v>
+      </c>
+      <c r="R6" s="1">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2336,8 +2485,14 @@
       <c r="P7" s="1">
         <v>3480</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1">
+        <v>3794</v>
+      </c>
+      <c r="R7" s="1">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2386,8 +2541,14 @@
       <c r="P8" s="1">
         <v>3534</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1">
+        <v>3785</v>
+      </c>
+      <c r="R8" s="1">
+        <v>3781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2436,8 +2597,14 @@
       <c r="P9" s="1">
         <v>3515</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1">
+        <v>3789</v>
+      </c>
+      <c r="R9" s="1">
+        <v>3788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2486,8 +2653,14 @@
       <c r="P10" s="1">
         <v>3515</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1">
+        <v>3778</v>
+      </c>
+      <c r="R10" s="1">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2536,8 +2709,14 @@
       <c r="P11" s="1">
         <v>3491</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1">
+        <v>3785</v>
+      </c>
+      <c r="R11" s="1">
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2598,11 +2777,19 @@
         <v>3749.3</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" ref="P12" si="3">AVERAGE(P2:P11)</f>
+        <f t="shared" ref="P12:Q12" si="3">AVERAGE(P2:P11)</f>
         <v>3507.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q12" s="3">
+        <f t="shared" si="3"/>
+        <v>3776.2</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" ref="R12" si="4">AVERAGE(R2:R11)</f>
+        <v>3794.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2611,63 +2798,71 @@
         <v>509.12222222222226</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="C13:G13" si="4">_xlfn.VAR.S(C2:C11)</f>
+        <f t="shared" ref="C13:G13" si="5">_xlfn.VAR.S(C2:C11)</f>
         <v>322.40000000000003</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>458.88888888888891</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>272.98888888888888</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>526.44444444444446</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1115.7777777777778</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13:M13" si="5">_xlfn.VAR.S(H2:H11)</f>
+        <f t="shared" ref="H13:M13" si="6">_xlfn.VAR.S(H2:H11)</f>
         <v>1531.377777777778</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>302.45555555555558</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1650.0111111111112</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3637.9555555555553</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1166.0444444444447</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>928.04444444444437</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" ref="N13:O13" si="6">_xlfn.VAR.S(N2:N11)</f>
+        <f t="shared" ref="N13:O13" si="7">_xlfn.VAR.S(N2:N11)</f>
         <v>179.65555555555557</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>323.12222222222226</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" ref="P13" si="7">_xlfn.VAR.S(P2:P11)</f>
+        <f t="shared" ref="P13:Q13" si="8">_xlfn.VAR.S(P2:P11)</f>
         <v>313.34444444444449</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3">
+        <f t="shared" si="8"/>
+        <v>149.51111111111112</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" ref="R13" si="9">_xlfn.VAR.S(R2:R11)</f>
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2691,47 +2886,55 @@
         <v>0.99999994274217585</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" ref="G14" si="8">1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
+        <f t="shared" ref="G14" si="10">1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
         <v>0.99999977450891742</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14:P14" si="9">1-_xlfn.T.TEST(G2:G11,H2:H11,2,3)</f>
+        <f t="shared" ref="H14:R14" si="11">1-_xlfn.T.TEST(G2:G11,H2:H11,2,3)</f>
         <v>1</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.99981320279925834</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.98922245269585052</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.99993237234027643</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.99999999997082467</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.999999999999999</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.99999999999999989</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="11"/>
+        <v>0.99903439244456249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2739,63 +2942,71 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:G15" si="10">B12/C12</f>
+        <f t="shared" ref="C15:G15" si="12">B12/C12</f>
         <v>1.0128558192206722</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0181865828092242</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0029041117491688</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0087354188759279</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.98562842957930497</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15" si="11">G12/H12</f>
+        <f t="shared" ref="H15" si="13">G12/H12</f>
         <v>1.1869242936451323</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ref="I15" si="12">H12/I12</f>
+        <f t="shared" ref="I15" si="14">H12/I12</f>
         <v>1.0111168603101433</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15" si="13">I12/J12</f>
+        <f t="shared" ref="J15" si="15">I12/J12</f>
         <v>1.0066291017567119</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" ref="K15" si="14">J12/K12</f>
+        <f t="shared" ref="K15" si="16">J12/K12</f>
         <v>1.2466451536736058</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" ref="L15" si="15">K12/L12</f>
+        <f t="shared" ref="L15" si="17">K12/L12</f>
         <v>1.0245131637301939</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15:P15" si="16">L12/M12</f>
+        <f t="shared" ref="M15:R15" si="18">L12/M12</f>
         <v>1.1849321612841583</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.0582673980636517</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.0551036193422771</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.0688770419363116</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1">
+        <f t="shared" si="18"/>
+        <v>0.92889677453524711</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="18"/>
+        <v>0.99512477929744114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2858,10 +3069,18 @@
         <f>B12/P12</f>
         <v>2.2438349915899307</v>
       </c>
+      <c r="Q16" s="1">
+        <f>B12/Q12</f>
+        <v>2.0842910862772102</v>
+      </c>
+      <c r="R16" s="1">
+        <f>B12/R12</f>
+        <v>2.0741297072232325</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:P16">
+  <conditionalFormatting sqref="B15:R16">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Make tls_vertex_cache as default. Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="135" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2175" yWindow="135" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +134,14 @@
   </si>
   <si>
     <t>v1469</t>
+  </si>
+  <si>
+    <t>v1475</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1475</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -632,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1033,15 +1041,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="K7" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1099,8 +1107,11 @@
       <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1158,8 +1169,11 @@
       <c r="S2" s="1">
         <v>4586</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T2" s="1">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1217,8 +1231,11 @@
       <c r="S3" s="1">
         <v>4591</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T3" s="1">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1276,8 +1293,11 @@
       <c r="S4" s="1">
         <v>4595</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T4" s="1">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1335,8 +1355,11 @@
       <c r="S5" s="1">
         <v>4580</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T5" s="1">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1394,8 +1417,11 @@
       <c r="S6" s="1">
         <v>4574</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T6" s="1">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1453,8 +1479,11 @@
       <c r="S7" s="1">
         <v>4595</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T7" s="1">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1512,8 +1541,11 @@
       <c r="S8" s="1">
         <v>4565</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T8" s="1">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1571,8 +1603,11 @@
       <c r="S9" s="1">
         <v>4584</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T9" s="1">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1630,8 +1665,11 @@
       <c r="S10" s="1">
         <v>4568</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T10" s="1">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1689,8 +1727,11 @@
       <c r="S11" s="1">
         <v>4581</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T11" s="1">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1766,8 +1807,12 @@
         <f t="shared" si="6"/>
         <v>4581.8999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T12" s="3">
+        <f t="shared" ref="T12" si="7">AVERAGE(T2:T11)</f>
+        <v>4551.8999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1776,75 +1821,79 @@
         <v>1875.377777777778</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="C13:G13" si="7">_xlfn.VAR.S(C2:C11)</f>
+        <f t="shared" ref="C13:G13" si="8">_xlfn.VAR.S(C2:C11)</f>
         <v>1924.1777777777779</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13" si="8">_xlfn.VAR.S(D2:D11)</f>
+        <f t="shared" ref="D13" si="9">_xlfn.VAR.S(D2:D11)</f>
         <v>682.01111111111118</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1472.3222222222223</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1224.4000000000005</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>704.48888888888894</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13:M13" si="9">_xlfn.VAR.S(H2:H11)</f>
+        <f t="shared" ref="H13:M13" si="10">_xlfn.VAR.S(H2:H11)</f>
         <v>7530.9333333333325</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1657.377777777778</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>250.45555555555561</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1827.8222222222223</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>411.51111111111118</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>421.51111111111118</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" ref="N13:O13" si="10">_xlfn.VAR.S(N2:N11)</f>
+        <f t="shared" ref="N13:O13" si="11">_xlfn.VAR.S(N2:N11)</f>
         <v>183.56666666666669</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>194.23333333333335</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" ref="P13:Q13" si="11">_xlfn.VAR.S(P2:P11)</f>
+        <f t="shared" ref="P13:Q13" si="12">_xlfn.VAR.S(P2:P11)</f>
         <v>1109.5111111111109</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1315.5666666666666</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" ref="R13:S13" si="12">_xlfn.VAR.S(R2:R11)</f>
+        <f t="shared" ref="R13:S13" si="13">_xlfn.VAR.S(R2:R11)</f>
         <v>48.4</v>
       </c>
       <c r="S13" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>110.32222222222222</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T13" s="3">
+        <f t="shared" ref="T13" si="14">_xlfn.VAR.S(T2:T11)</f>
+        <v>669.87777777777785</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1856,71 +1905,75 @@
         <v>0.9999999869691466</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:S14" si="13">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
+        <f t="shared" ref="D14:T14" si="15">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999999999889</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999999999867</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999993108443863</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999999999278</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.96439230163877454</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999936755718299</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99959879047769007</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999624907909</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999999745648</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99999999999957156</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T14" s="1">
+        <f t="shared" si="15"/>
+        <v>0.99462714415732034</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1928,75 +1981,79 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:S15" si="14">B12/C12</f>
+        <f t="shared" ref="C15:T15" si="16">B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0499883346150856</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.104887293419005</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.042385700921558</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.98759632017612842</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.2051549322467545</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.9916369103551963</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0159790923302743</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0085573983583276</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1484215182175044</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0354955058109578</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1168694150934348</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0806744173994161</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0304211613086973</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0483512792281711</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1257300113440611</v>
       </c>
       <c r="S15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0389139876470461</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="T15" s="1">
+        <f t="shared" si="16"/>
+        <v>1.0065906544519871</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2071,10 +2128,14 @@
         <f>B12/S12</f>
         <v>2.6935114253912134</v>
       </c>
+      <c r="T16" s="1">
+        <f>B12/T12</f>
+        <v>2.7112634284584463</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:S16">
+  <conditionalFormatting sqref="B15:T16">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2092,15 +2153,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2155,8 +2216,11 @@
       <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2211,8 +2275,11 @@
       <c r="R2" s="1">
         <v>3791</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S2" s="1">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2267,8 +2334,11 @@
       <c r="R3" s="1">
         <v>3795</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S3" s="1">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2323,8 +2393,11 @@
       <c r="R4" s="1">
         <v>3796</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S4" s="1">
+        <v>3689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2379,8 +2452,11 @@
       <c r="R5" s="1">
         <v>3798</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S5" s="1">
+        <v>3687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2435,8 +2511,11 @@
       <c r="R6" s="1">
         <v>3809</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S6" s="1">
+        <v>3704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2491,8 +2570,11 @@
       <c r="R7" s="1">
         <v>3795</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S7" s="1">
+        <v>3722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2547,8 +2629,11 @@
       <c r="R8" s="1">
         <v>3781</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S8" s="1">
+        <v>3718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2603,8 +2688,11 @@
       <c r="R9" s="1">
         <v>3788</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S9" s="1">
+        <v>3702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2659,8 +2747,11 @@
       <c r="R10" s="1">
         <v>3798</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S10" s="1">
+        <v>3726</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2715,8 +2806,11 @@
       <c r="R11" s="1">
         <v>3796</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S11" s="1">
+        <v>3711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2785,11 +2879,15 @@
         <v>3776.2</v>
       </c>
       <c r="R12" s="3">
-        <f t="shared" ref="R12" si="4">AVERAGE(R2:R11)</f>
+        <f t="shared" ref="R12:S12" si="4">AVERAGE(R2:R11)</f>
         <v>3794.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S12" s="3">
+        <f t="shared" si="4"/>
+        <v>3712.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2858,11 +2956,15 @@
         <v>149.51111111111112</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" ref="R13" si="9">_xlfn.VAR.S(R2:R11)</f>
+        <f t="shared" ref="R13:S13" si="9">_xlfn.VAR.S(R2:R11)</f>
         <v>52.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S13" s="3">
+        <f t="shared" si="9"/>
+        <v>286.72222222222223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2890,7 +2992,7 @@
         <v>0.99999977450891742</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14:R14" si="11">1-_xlfn.T.TEST(G2:G11,H2:H11,2,3)</f>
+        <f t="shared" ref="H14:S14" si="11">1-_xlfn.T.TEST(G2:G11,H2:H11,2,3)</f>
         <v>1</v>
       </c>
       <c r="I14" s="1">
@@ -2933,8 +3035,12 @@
         <f t="shared" si="11"/>
         <v>0.99903439244456249</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S14" s="1">
+        <f t="shared" si="11"/>
+        <v>0.99999999365129755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2982,7 +3088,7 @@
         <v>1.0245131637301939</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15:R15" si="18">L12/M12</f>
+        <f t="shared" ref="M15:S15" si="18">L12/M12</f>
         <v>1.1849321612841583</v>
       </c>
       <c r="N15" s="1">
@@ -3005,8 +3111,12 @@
         <f t="shared" si="18"/>
         <v>0.99512477929744114</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="S15" s="1">
+        <f t="shared" si="18"/>
+        <v>1.022141414141414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3077,10 +3187,14 @@
         <f>B12/R12</f>
         <v>2.0741297072232325</v>
       </c>
+      <c r="S16" s="1">
+        <f>B12/S12</f>
+        <v>2.1200538720538722</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B15:R16">
+  <conditionalFormatting sqref="B15:S16">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update issue 226 Print profiling on the end of benchmark. All samples ported to sample_app framework.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance_A45.xlsx
+++ b/doc/contents/materials/PipelinePerformance_A45.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="135" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="2175" yWindow="135" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
     <sheet name="Sponza" sheetId="5" r:id="rId2"/>
     <sheet name="ComplexMesh" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -148,17 +148,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,9 +204,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -293,12 +307,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -340,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,12 +607,12 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,7 +633,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -637,7 +654,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -658,7 +675,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -679,7 +696,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -700,7 +717,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -721,7 +738,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -742,7 +759,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -763,7 +780,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -784,7 +801,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -805,7 +822,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -826,7 +843,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -855,7 +872,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -884,7 +901,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -912,7 +929,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -940,7 +957,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -989,13 +1006,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1083,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1119,7 +1145,7 @@
         <v>4543</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1181,7 +1207,7 @@
         <v>4547</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1243,7 +1269,7 @@
         <v>4528</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1305,7 +1331,7 @@
         <v>4592</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1367,7 +1393,7 @@
         <v>4597</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1429,7 +1455,7 @@
         <v>4573</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1491,7 +1517,7 @@
         <v>4542</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1553,7 +1579,7 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1615,7 +1641,7 @@
         <v>4536</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1677,7 +1703,7 @@
         <v>4531</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1758,323 +1784,323 @@
         <v>4551.8999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:20" s="8" customFormat="1">
+      <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <f>_xlfn.VAR.S(B2:B11)</f>
         <v>1875.377777777778</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="7">
         <f t="shared" ref="C13:G13" si="8">_xlfn.VAR.S(C2:C11)</f>
         <v>1924.1777777777779</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="7">
         <f t="shared" ref="D13" si="9">_xlfn.VAR.S(D2:D11)</f>
         <v>682.01111111111118</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="7">
         <f t="shared" si="8"/>
         <v>1472.3222222222223</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="7">
         <f t="shared" si="8"/>
         <v>1224.4000000000005</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="7">
         <f t="shared" si="8"/>
         <v>704.48888888888894</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="7">
         <f t="shared" ref="H13:M13" si="10">_xlfn.VAR.S(H2:H11)</f>
         <v>7530.9333333333325</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="7">
         <f t="shared" si="10"/>
         <v>1657.377777777778</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="7">
         <f t="shared" si="10"/>
         <v>250.45555555555561</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="7">
         <f t="shared" si="10"/>
         <v>1827.8222222222223</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="7">
         <f t="shared" si="10"/>
         <v>411.51111111111118</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="7">
         <f t="shared" si="10"/>
         <v>421.51111111111118</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="7">
         <f t="shared" ref="N13:O13" si="11">_xlfn.VAR.S(N2:N11)</f>
         <v>183.56666666666669</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="7">
         <f t="shared" si="11"/>
         <v>194.23333333333335</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="7">
         <f t="shared" ref="P13:Q13" si="12">_xlfn.VAR.S(P2:P11)</f>
         <v>1109.5111111111109</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="7">
         <f t="shared" si="12"/>
         <v>1315.5666666666666</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="7">
         <f t="shared" ref="R13:S13" si="13">_xlfn.VAR.S(R2:R11)</f>
         <v>48.4</v>
       </c>
-      <c r="S13" s="3">
+      <c r="S13" s="7">
         <f t="shared" si="13"/>
         <v>110.32222222222222</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="7">
         <f t="shared" ref="T13" si="14">_xlfn.VAR.S(T2:T11)</f>
         <v>669.87777777777785</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:20" s="5" customFormat="1">
+      <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
         <v>0.9999999869691466</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <f t="shared" ref="D14:T14" si="15">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
         <v>0.99999999999999889</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999999999867</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999993108443863</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999999999278</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="4">
         <f t="shared" si="15"/>
         <v>0.96439230163877454</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999936755718299</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="4">
         <f t="shared" si="15"/>
         <v>0.99959879047769007</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999999999956</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999624907909</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999999745648</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="4">
         <f t="shared" si="15"/>
         <v>0.99999999999957156</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="4">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="4">
         <f t="shared" si="15"/>
         <v>0.99462714415732034</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:20" s="5" customFormat="1">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <f t="shared" ref="C15:T15" si="16">B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <f t="shared" si="16"/>
         <v>1.0499883346150856</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <f t="shared" si="16"/>
         <v>1.104887293419005</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <f t="shared" si="16"/>
         <v>1.042385700921558</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <f t="shared" si="16"/>
         <v>0.98759632017612842</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <f t="shared" si="16"/>
         <v>1.2051549322467545</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="4">
         <f t="shared" si="16"/>
         <v>0.9916369103551963</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="4">
         <f t="shared" si="16"/>
         <v>1.0159790923302743</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="4">
         <f t="shared" si="16"/>
         <v>1.0085573983583276</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="4">
         <f t="shared" si="16"/>
         <v>1.1484215182175044</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="4">
         <f t="shared" si="16"/>
         <v>1.0354955058109578</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="4">
         <f t="shared" si="16"/>
         <v>1.1168694150934348</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="4">
         <f t="shared" si="16"/>
         <v>1.0806744173994161</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="4">
         <f t="shared" si="16"/>
         <v>1.0304211613086973</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q15" s="4">
         <f t="shared" si="16"/>
         <v>1.0483512792281711</v>
       </c>
-      <c r="R15" s="1">
+      <c r="R15" s="4">
         <f t="shared" si="16"/>
         <v>1.1257300113440611</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="4">
         <f t="shared" si="16"/>
         <v>1.0389139876470461</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15" s="4">
         <f t="shared" si="16"/>
         <v>1.0065906544519871</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:20" s="5" customFormat="1">
+      <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f>B12/C12</f>
         <v>1.0156527750345643</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <f>B12/D12</f>
         <v>1.0664235658057324</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <f>B12/E12</f>
         <v>1.1782778472613398</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <f>B12/F12</f>
         <v>1.2282199796978561</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <f>B12/G12</f>
         <v>1.212985532316402</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <f>B12/H12</f>
         <v>1.4618354970150669</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <f>B12/I12</f>
         <v>1.4496100357075736</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="4">
         <f>B12/J12</f>
         <v>1.4727734883110373</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="4">
         <f>B12/K12</f>
         <v>1.4853765977420985</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="4">
         <f>B12/L12</f>
         <v>1.7058384475037318</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="4">
         <f>B12/M12</f>
         <v>1.7663880460296559</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="4">
         <f>B12/N12</f>
         <v>1.9728247837971771</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="4">
         <f>B12/O12</f>
         <v>2.1319812738611432</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="4">
         <f>B12/P12</f>
         <v>2.1968386201003951</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q16" s="4">
         <f>B12/Q12</f>
         <v>2.3030585776400994</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16" s="4">
         <f>B12/R12</f>
         <v>2.5926221587328264</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="4">
         <f>B12/S12</f>
         <v>2.6935114253912134</v>
       </c>
-      <c r="T16" s="1">
+      <c r="T16" s="4">
         <f>B12/T12</f>
         <v>2.7112634284584463</v>
       </c>
@@ -2101,13 +2127,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2166,7 +2192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2225,7 +2251,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2284,7 +2310,7 @@
         <v>3728</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2343,7 +2369,7 @@
         <v>3689</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2402,7 +2428,7 @@
         <v>3687</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2461,7 +2487,7 @@
         <v>3704</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2520,7 +2546,7 @@
         <v>3722</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2579,7 +2605,7 @@
         <v>3718</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2638,7 +2664,7 @@
         <v>3702</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2697,7 +2723,7 @@
         <v>3726</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2756,7 +2782,7 @@
         <v>3711</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2833,7 +2859,7 @@
         <v>3712.5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2910,7 +2936,7 @@
         <v>286.72222222222223</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2986,7 +3012,7 @@
         <v>0.99999999365129755</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3062,7 +3088,7 @@
         <v>1.022141414141414</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>